<commit_message>
laptop added sound module and config
</commit_message>
<xml_diff>
--- a/project docs/Robot's expences.xlsx
+++ b/project docs/Robot's expences.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>expences for robot :</t>
   </si>
@@ -79,10 +79,25 @@
     <t>adafruit 16chan pwm board</t>
   </si>
   <si>
-    <t>½ price shipping</t>
+    <t>½ price for shipping</t>
   </si>
   <si>
     <t>microphone usb</t>
+  </si>
+  <si>
+    <t>capacitor</t>
+  </si>
+  <si>
+    <t>usb expander</t>
+  </si>
+  <si>
+    <t>Soldering-iron holder</t>
+  </si>
+  <si>
+    <t>lan cable</t>
+  </si>
+  <si>
+    <t>lan socket</t>
   </si>
 </sst>
 </file>
@@ -144,7 +159,7 @@
       <sz val="9"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -155,6 +170,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -192,7 +213,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -217,6 +238,14 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="3" fontId="0" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -230,6 +259,10 @@
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -250,17 +283,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A20" activeCellId="0" pane="topLeft" sqref="A20:B20"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A7" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B27" activeCellId="0" pane="topLeft" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.2874493927125"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.5465587044534"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.331983805668"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.53441295546559"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.5668016194332"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.53441295546559"/>
@@ -277,7 +310,7 @@
       </c>
       <c r="E2" s="0" t="n">
         <f aca="false">SUM(B:B)</f>
-        <v>416.94</v>
+        <v>456.44</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
@@ -343,14 +376,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="10">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="5" t="n">
+      <c r="B10" s="7" t="n">
         <v>0.5</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="11">
@@ -370,7 +400,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="13">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="1" t="n">
@@ -379,7 +409,7 @@
       <c r="E13" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="14">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="1" t="n">
@@ -388,7 +418,7 @@
       <c r="E14" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="15">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="5" t="n">
@@ -400,16 +430,16 @@
       <c r="E15" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="16">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="8" t="n">
+      <c r="B16" s="10" t="n">
         <v>28.68</v>
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="17">
-      <c r="A17" s="6" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="17">
+      <c r="A17" s="8" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="1" t="n">
@@ -421,7 +451,7 @@
       <c r="A18" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="9" t="n">
+      <c r="B18" s="11" t="n">
         <v>71.63</v>
       </c>
       <c r="C18" s="0" t="s">
@@ -442,6 +472,54 @@
       </c>
       <c r="B20" s="1" t="n">
         <v>1.5</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="21">
+      <c r="A21" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="1" t="n">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="22">
+      <c r="A22" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="1" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="23">
+      <c r="A23" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="1" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="24">
+      <c r="A24" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="5" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="25">
+      <c r="A25" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="1" t="n">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="26">
+      <c r="A26" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="1" t="n">
+        <v>1.9</v>
       </c>
     </row>
   </sheetData>
@@ -463,7 +541,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="A20:B20 A1"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -489,7 +567,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="A20:B20 A1"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>